<commit_message>
Add files via CLI
</commit_message>
<xml_diff>
--- a/Assignment-01-Rubric.xlsx
+++ b/Assignment-01-Rubric.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t>If any of these are not completed, you will receive a 0 on the Assignment</t>
   </si>
@@ -20,6 +20,26 @@
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Attend the Discussion Section meeting for the </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>first TWO weeks</t>
+    </r>
+  </si>
+  <si>
+    <t>Review the assignment with your DL, and hit the "Submit" button under the supervision of your DL</t>
   </si>
   <si>
     <t>Zipped Submission Folder</t>
@@ -126,91 +146,19 @@
     <t>2 Pts</t>
   </si>
   <si>
-    <t>Includes screenshot of the CSC 210 File Manager</t>
+    <t>Includes screenshot of Code_Referrence directory in CSC 215 File Manager</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">Includes screenshot of </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Code_Referrence</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> directory in CSC 215 File Manager</t>
-    </r>
+    <t>Includes screenshot of Tutorials directory in CSC 215 File Manager</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">Includes screenshot of </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Tutorials</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> directory in CSC 215 File Manager</t>
-    </r>
+    <t>Includes screenshot of WEEK-01 directory in CSC 215 File Manager</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">Includes screenshot of </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>WEEK-01</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> directory in CSC 215 File Manager</t>
-    </r>
+    <t xml:space="preserve">Includes screenshot of very last offered CSC210 File Manager </t>
   </si>
   <si>
-    <t>Includes screenshot of a different directory of your choice in CSC 215 File Manager</t>
+    <t xml:space="preserve">Includes screenshot of previous CSC 215 File Manager </t>
   </si>
   <si>
     <t>Part C</t>
@@ -382,7 +330,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -404,7 +352,7 @@
     <font>
       <b/>
       <sz val="11.0"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -415,11 +363,20 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font/>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
       <b/>
       <sz val="12.0"/>
@@ -432,11 +389,6 @@
       <sz val="13.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
     </font>
     <font>
       <b/>
@@ -483,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="37">
     <border/>
     <border>
       <left style="thick">
@@ -502,12 +454,48 @@
       </left>
     </border>
     <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
       <top style="thick">
         <color rgb="FF000000"/>
       </top>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thick">
@@ -542,6 +530,9 @@
       </top>
     </border>
     <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
@@ -581,40 +572,10 @@
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -639,20 +600,6 @@
       <top style="thick">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <right style="thick">
@@ -890,7 +837,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -919,77 +866,83 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="13" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="5" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="13" fillId="5" fontId="10" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="14" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1001,190 +954,190 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="13" fillId="0" fontId="10" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="20" fillId="5" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="19" fillId="5" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="18" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="22" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="23" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="22" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="24" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="23" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="25" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="26" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="25" fillId="0" fontId="10" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="27" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="26" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="28" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="27" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="29" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="28" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="30" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="29" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="31" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="30" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="32" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="31" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="33" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="32" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="34" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="33" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="35" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="34" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="36" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="35" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="37" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="36" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="24" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="23" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1401,16 +1354,16 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2.0" ySplit="7.0" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2.0" ySplit="9.0" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1" pane="topRight"/>
-      <selection activeCell="A8" sqref="A8" pane="bottomLeft"/>
-      <selection activeCell="C8" sqref="C8" pane="bottomRight"/>
+      <selection activeCell="A10" sqref="A10" pane="bottomLeft"/>
+      <selection activeCell="C10" sqref="C10" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="4.0"/>
-    <col customWidth="1" min="2" max="2" width="74.25"/>
+    <col customWidth="1" min="2" max="2" width="76.5"/>
     <col customWidth="1" min="3" max="3" width="8.63"/>
     <col customWidth="1" min="4" max="4" width="17.13"/>
     <col customWidth="1" min="5" max="5" width="68.75"/>
@@ -1484,8 +1437,8 @@
         <v>3</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -1510,12 +1463,12 @@
     </row>
     <row r="4">
       <c r="A4" s="1"/>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1540,12 +1493,12 @@
     </row>
     <row r="5">
       <c r="A5" s="1"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="14"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1570,12 +1523,12 @@
     </row>
     <row r="6">
       <c r="A6" s="1"/>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1600,14 +1553,12 @@
     </row>
     <row r="7">
       <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>8</v>
-      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1632,8 +1583,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
       <c r="F8" s="2"/>
@@ -1662,8 +1615,12 @@
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1687,15 +1644,11 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1719,17 +1672,11 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="23">
-        <v>1.0</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1753,15 +1700,15 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="27"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1785,17 +1732,17 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="23">
-        <v>2.0</v>
+      <c r="A13" s="25">
+        <v>1.0</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="28">
-        <v>0.4</v>
+      <c r="C13" s="26">
+        <v>0.5</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1819,15 +1766,15 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="23"/>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="28">
-        <v>0.3</v>
+      <c r="C14" s="30">
+        <v>0.5</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="26"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1851,15 +1798,17 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="28">
-        <v>0.3</v>
+      <c r="C15" s="30">
+        <v>0.4</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="28"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1883,17 +1832,15 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="28">
-        <v>1.0</v>
+      <c r="C16" s="30">
+        <v>0.3</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="28"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1917,17 +1864,15 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="32">
-        <v>4.0</v>
-      </c>
-      <c r="B17" s="15" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="33">
-        <v>1.0</v>
+      <c r="C17" s="30">
+        <v>0.3</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1951,19 +1896,17 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="36"/>
-      <c r="B18" s="37" t="s">
+      <c r="A18" s="29">
+        <v>3.0</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="3">
-        <f t="shared" ref="C18:D18" si="1">sum(C11:C17)</f>
-        <v>4</v>
+      <c r="C18" s="30">
+        <v>1.0</v>
       </c>
-      <c r="D18" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="4"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="33"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1987,11 +1930,17 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="4"/>
+      <c r="A19" s="34">
+        <v>4.0</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -2015,10 +1964,18 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="1"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" ref="C20:D20" si="1">sum(C13:C19)</f>
+        <v>4</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -2043,15 +2000,11 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="41"/>
-      <c r="E21" s="22"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -2075,17 +2028,11 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="43">
-        <v>0.4</v>
-      </c>
-      <c r="D22" s="44"/>
-      <c r="E22" s="30"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -2109,17 +2056,15 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="45">
-        <v>2.0</v>
+      <c r="A23" s="40"/>
+      <c r="B23" s="41" t="s">
+        <v>21</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="C23" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="43">
-        <v>0.4</v>
-      </c>
-      <c r="D23" s="47"/>
-      <c r="E23" s="48"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -2143,17 +2088,17 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="45">
-        <v>3.0</v>
+      <c r="A24" s="29">
+        <v>1.0</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="45">
         <v>0.4</v>
       </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="48"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="32"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -2177,17 +2122,17 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25">
-      <c r="A25" s="45">
-        <v>4.0</v>
+      <c r="A25" s="47">
+        <v>2.0</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="45">
         <v>0.4</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="48"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="50"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -2211,18 +2156,18 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26">
-      <c r="A26" s="32">
-        <v>5.0</v>
+      <c r="A26" s="47">
+        <v>3.0</v>
       </c>
       <c r="B26" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="52">
+      <c r="C26" s="45">
         <v>0.4</v>
       </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="54"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -2245,19 +2190,17 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27">
-      <c r="A27" s="36"/>
-      <c r="B27" s="37" t="s">
-        <v>18</v>
+      <c r="A27" s="47">
+        <v>4.0</v>
       </c>
-      <c r="C27" s="3">
-        <f>SUM(C22:C26)</f>
-        <v>2</v>
+      <c r="B27" s="51" t="s">
+        <v>26</v>
       </c>
-      <c r="D27" s="55">
-        <f>sum(D22:D26)</f>
-        <v>0</v>
+      <c r="C27" s="45">
+        <v>0.4</v>
       </c>
-      <c r="E27" s="56"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="50"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -2281,12 +2224,18 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="2"/>
+      <c r="A28" s="34">
+        <v>5.0</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="54">
+        <v>0.4</v>
+      </c>
+      <c r="D28" s="52"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -2309,11 +2258,19 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="4"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="3">
+        <f>SUM(C24:C28)</f>
+        <v>2</v>
+      </c>
+      <c r="D29" s="57">
+        <f>sum(D24:D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="58"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -2337,15 +2294,11 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="38"/>
-      <c r="B30" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="22"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="4"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -2369,17 +2322,11 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31">
-      <c r="A31" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="B31" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="D31" s="44"/>
-      <c r="E31" s="30"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="4"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -2403,17 +2350,15 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32">
-      <c r="A32" s="27">
-        <v>2.0</v>
+      <c r="A32" s="40"/>
+      <c r="B32" s="40" t="s">
+        <v>28</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="C32" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="48"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2437,17 +2382,17 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="23">
-        <v>3.0</v>
+      <c r="A33" s="29">
+        <v>1.0</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="28">
-        <v>2.0</v>
+      <c r="C33" s="26">
+        <v>1.0</v>
       </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="53"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -2471,15 +2416,17 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="32"/>
-      <c r="B34" s="51" t="s">
+      <c r="A34" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="B34" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="33">
-        <v>1.0</v>
+      <c r="C34" s="30">
+        <v>2.0</v>
       </c>
-      <c r="D34" s="59"/>
-      <c r="E34" s="60"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2503,19 +2450,17 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35">
-      <c r="A35" s="36"/>
-      <c r="B35" s="37" t="s">
-        <v>18</v>
+      <c r="A35" s="25">
+        <v>3.0</v>
       </c>
-      <c r="C35" s="3">
-        <f>SUM(C31:C34)</f>
-        <v>6</v>
+      <c r="B35" s="60" t="s">
+        <v>32</v>
       </c>
-      <c r="D35" s="1">
-        <f>sum(D31:D34)</f>
-        <v>0</v>
+      <c r="C35" s="30">
+        <v>2.0</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="55"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -2539,11 +2484,15 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="4"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="D36" s="61"/>
+      <c r="E36" s="62"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2567,10 +2516,18 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="1"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="3">
+        <f>SUM(C33:C36)</f>
+        <v>6</v>
+      </c>
+      <c r="D37" s="1">
+        <f>sum(D33:D36)</f>
+        <v>0</v>
+      </c>
       <c r="E37" s="4"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2595,15 +2552,11 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="38"/>
-      <c r="B38" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="21"/>
-      <c r="E38" s="22"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="4"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -2627,15 +2580,11 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39">
-      <c r="A39" s="23"/>
-      <c r="B39" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="24">
-        <v>0.25</v>
-      </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="26"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="4"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -2659,15 +2608,15 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40">
-      <c r="A40" s="23"/>
-      <c r="B40" s="58" t="s">
+      <c r="A40" s="40"/>
+      <c r="B40" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="26"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="24"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -2691,15 +2640,15 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41">
-      <c r="A41" s="27"/>
-      <c r="B41" s="58" t="s">
+      <c r="A41" s="25"/>
+      <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="28">
+      <c r="C41" s="26">
         <v>0.25</v>
       </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="30"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="28"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -2723,15 +2672,15 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42">
-      <c r="A42" s="23"/>
-      <c r="B42" s="58" t="s">
+      <c r="A42" s="25"/>
+      <c r="B42" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="28">
-        <v>0.25</v>
+      <c r="C42" s="30">
+        <v>0.5</v>
       </c>
-      <c r="D42" s="29"/>
-      <c r="E42" s="26"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="28"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -2755,15 +2704,15 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43">
-      <c r="A43" s="23"/>
-      <c r="B43" s="58" t="s">
+      <c r="A43" s="29"/>
+      <c r="B43" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="28">
-        <v>0.5</v>
+      <c r="C43" s="30">
+        <v>0.25</v>
       </c>
-      <c r="D43" s="29"/>
-      <c r="E43" s="26"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="32"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2787,15 +2736,15 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44">
-      <c r="A44" s="27"/>
-      <c r="B44" s="58" t="s">
+      <c r="A44" s="25"/>
+      <c r="B44" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="28">
+      <c r="C44" s="30">
         <v>0.25</v>
       </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="30"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="28"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2819,15 +2768,15 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45">
-      <c r="A45" s="23"/>
-      <c r="B45" s="58" t="s">
+      <c r="A45" s="25"/>
+      <c r="B45" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="28">
-        <v>0.25</v>
+      <c r="C45" s="30">
+        <v>0.5</v>
       </c>
-      <c r="D45" s="29"/>
-      <c r="E45" s="26"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="28"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -2851,15 +2800,15 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46">
-      <c r="A46" s="23"/>
-      <c r="B46" s="58" t="s">
+      <c r="A46" s="29"/>
+      <c r="B46" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="28">
-        <v>0.5</v>
+      <c r="C46" s="30">
+        <v>0.25</v>
       </c>
-      <c r="D46" s="29"/>
-      <c r="E46" s="26"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="32"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -2883,15 +2832,15 @@
       <c r="Z46" s="2"/>
     </row>
     <row r="47">
-      <c r="A47" s="61"/>
-      <c r="B47" s="62" t="s">
+      <c r="A47" s="25"/>
+      <c r="B47" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="33">
+      <c r="C47" s="30">
         <v>0.25</v>
       </c>
-      <c r="D47" s="34"/>
-      <c r="E47" s="60"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="28"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2915,19 +2864,15 @@
       <c r="Z47" s="2"/>
     </row>
     <row r="48">
-      <c r="A48" s="36"/>
-      <c r="B48" s="37" t="s">
-        <v>18</v>
+      <c r="A48" s="25"/>
+      <c r="B48" s="60" t="s">
+        <v>43</v>
       </c>
-      <c r="C48" s="3">
-        <f>SUM(C39:C47)</f>
-        <v>3</v>
+      <c r="C48" s="30">
+        <v>0.5</v>
       </c>
-      <c r="D48" s="1">
-        <f>sum(D39:D46)</f>
-        <v>0</v>
-      </c>
-      <c r="E48" s="4"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="28"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -2951,11 +2896,15 @@
       <c r="Z48" s="2"/>
     </row>
     <row r="49">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="4"/>
+      <c r="A49" s="63"/>
+      <c r="B49" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="D49" s="36"/>
+      <c r="E49" s="62"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -2979,10 +2928,18 @@
       <c r="Z49" s="2"/>
     </row>
     <row r="50">
-      <c r="A50" s="1"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="1"/>
+      <c r="A50" s="38"/>
+      <c r="B50" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="3">
+        <f>SUM(C41:C49)</f>
+        <v>3</v>
+      </c>
+      <c r="D50" s="1">
+        <f>sum(D41:D48)</f>
+        <v>0</v>
+      </c>
       <c r="E50" s="4"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -3007,15 +2964,11 @@
       <c r="Z50" s="2"/>
     </row>
     <row r="51">
-      <c r="A51" s="38"/>
-      <c r="B51" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="C51" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="D51" s="41"/>
-      <c r="E51" s="22"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="4"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -3039,15 +2992,11 @@
       <c r="Z51" s="2"/>
     </row>
     <row r="52">
-      <c r="A52" s="27"/>
-      <c r="B52" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="D52" s="44"/>
-      <c r="E52" s="30"/>
+      <c r="A52" s="1"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="4"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -3071,15 +3020,15 @@
       <c r="Z52" s="2"/>
     </row>
     <row r="53">
-      <c r="A53" s="64"/>
+      <c r="A53" s="40"/>
       <c r="B53" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="66">
-        <v>1.0</v>
+      <c r="C53" s="42" t="s">
+        <v>35</v>
       </c>
-      <c r="D53" s="67"/>
-      <c r="E53" s="48"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="24"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -3103,15 +3052,15 @@
       <c r="Z53" s="2"/>
     </row>
     <row r="54">
-      <c r="A54" s="68"/>
-      <c r="B54" s="15" t="s">
+      <c r="A54" s="29"/>
+      <c r="B54" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="33">
+      <c r="C54" s="26">
         <v>1.0</v>
       </c>
-      <c r="D54" s="59"/>
-      <c r="E54" s="69"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="32"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -3135,19 +3084,15 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55">
-      <c r="A55" s="36"/>
-      <c r="B55" s="37" t="s">
-        <v>18</v>
+      <c r="A55" s="66"/>
+      <c r="B55" s="67" t="s">
+        <v>47</v>
       </c>
-      <c r="C55" s="3">
-        <f>SUM(C52:C54)</f>
-        <v>3</v>
+      <c r="C55" s="68">
+        <v>1.0</v>
       </c>
-      <c r="D55" s="1">
-        <f>sum(D52:D54)</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="4"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="50"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -3171,11 +3116,15 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="4"/>
+      <c r="A56" s="70"/>
+      <c r="B56" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="D56" s="61"/>
+      <c r="E56" s="71"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -3199,10 +3148,18 @@
       <c r="Z56" s="2"/>
     </row>
     <row r="57">
-      <c r="A57" s="1"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="1"/>
+      <c r="A57" s="38"/>
+      <c r="B57" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="3">
+        <f>SUM(C54:C56)</f>
+        <v>3</v>
+      </c>
+      <c r="D57" s="1">
+        <f>sum(D54:D56)</f>
+        <v>0</v>
+      </c>
       <c r="E57" s="4"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -3227,15 +3184,11 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58">
-      <c r="A58" s="38"/>
-      <c r="B58" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C58" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D58" s="41"/>
-      <c r="E58" s="22"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="4"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -3259,15 +3212,11 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59">
-      <c r="A59" s="23"/>
-      <c r="B59" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="C59" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="D59" s="44"/>
-      <c r="E59" s="26"/>
+      <c r="A59" s="1"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="4"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -3291,15 +3240,15 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60">
-      <c r="A60" s="23"/>
-      <c r="B60" s="70" t="s">
+      <c r="A60" s="40"/>
+      <c r="B60" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C60" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C60" s="71">
-        <v>0.5</v>
-      </c>
-      <c r="D60" s="50"/>
-      <c r="E60" s="26"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="24"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -3323,15 +3272,15 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61">
-      <c r="A61" s="23"/>
-      <c r="B61" s="70" t="s">
+      <c r="A61" s="25"/>
+      <c r="B61" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="C61" s="71">
+      <c r="C61" s="26">
         <v>1.0</v>
       </c>
-      <c r="D61" s="50"/>
-      <c r="E61" s="26"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="28"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -3355,15 +3304,15 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62">
-      <c r="A62" s="23"/>
-      <c r="B62" s="70" t="s">
+      <c r="A62" s="25"/>
+      <c r="B62" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="C62" s="71">
-        <v>1.0</v>
+      <c r="C62" s="73">
+        <v>0.5</v>
       </c>
-      <c r="D62" s="50"/>
-      <c r="E62" s="26"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="28"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -3387,15 +3336,15 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63">
-      <c r="A63" s="23"/>
-      <c r="B63" s="70" t="s">
+      <c r="A63" s="25"/>
+      <c r="B63" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="71">
+      <c r="C63" s="73">
         <v>1.0</v>
       </c>
-      <c r="D63" s="50"/>
-      <c r="E63" s="26"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="28"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -3419,15 +3368,15 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64">
-      <c r="A64" s="23"/>
-      <c r="B64" s="70" t="s">
+      <c r="A64" s="25"/>
+      <c r="B64" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="C64" s="71">
+      <c r="C64" s="73">
         <v>1.0</v>
       </c>
-      <c r="D64" s="50"/>
-      <c r="E64" s="26"/>
+      <c r="D64" s="52"/>
+      <c r="E64" s="28"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -3451,15 +3400,15 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65">
-      <c r="A65" s="23"/>
-      <c r="B65" s="70" t="s">
+      <c r="A65" s="25"/>
+      <c r="B65" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="C65" s="71">
+      <c r="C65" s="73">
         <v>1.0</v>
       </c>
-      <c r="D65" s="50"/>
-      <c r="E65" s="26"/>
+      <c r="D65" s="52"/>
+      <c r="E65" s="28"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -3483,15 +3432,15 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66">
-      <c r="A66" s="32"/>
-      <c r="B66" s="51" t="s">
+      <c r="A66" s="25"/>
+      <c r="B66" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="C66" s="33">
-        <v>0.5</v>
+      <c r="C66" s="73">
+        <v>1.0</v>
       </c>
-      <c r="D66" s="59"/>
-      <c r="E66" s="60"/>
+      <c r="D66" s="52"/>
+      <c r="E66" s="28"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
@@ -3515,19 +3464,15 @@
       <c r="Z66" s="2"/>
     </row>
     <row r="67">
-      <c r="A67" s="36"/>
-      <c r="B67" s="37" t="s">
-        <v>18</v>
+      <c r="A67" s="25"/>
+      <c r="B67" s="72" t="s">
+        <v>57</v>
       </c>
-      <c r="C67" s="3">
-        <f>SUM(C59:C66)</f>
-        <v>7</v>
+      <c r="C67" s="73">
+        <v>1.0</v>
       </c>
-      <c r="D67" s="1">
-        <f>sum(D59:D66)</f>
-        <v>0</v>
-      </c>
-      <c r="E67" s="4"/>
+      <c r="D67" s="52"/>
+      <c r="E67" s="28"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -3551,11 +3496,15 @@
       <c r="Z67" s="2"/>
     </row>
     <row r="68">
-      <c r="A68" s="36"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="4"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="D68" s="61"/>
+      <c r="E68" s="62"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -3579,10 +3528,18 @@
       <c r="Z68" s="2"/>
     </row>
     <row r="69">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="1"/>
+      <c r="A69" s="38"/>
+      <c r="B69" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="3">
+        <f>SUM(C61:C68)</f>
+        <v>7</v>
+      </c>
+      <c r="D69" s="1">
+        <f>sum(D61:D68)</f>
+        <v>0</v>
+      </c>
       <c r="E69" s="4"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -3608,14 +3565,10 @@
     </row>
     <row r="70">
       <c r="A70" s="38"/>
-      <c r="B70" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="C70" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D70" s="63"/>
-      <c r="E70" s="72"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="4"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -3639,149 +3592,145 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71">
-      <c r="A71" s="73">
+      <c r="A71" s="1"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="2"/>
+      <c r="S71" s="2"/>
+      <c r="T71" s="2"/>
+      <c r="U71" s="2"/>
+      <c r="V71" s="2"/>
+      <c r="W71" s="2"/>
+      <c r="X71" s="2"/>
+      <c r="Y71" s="2"/>
+      <c r="Z71" s="2"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="40"/>
+      <c r="B72" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C72" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" s="65"/>
+      <c r="E72" s="74"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="2"/>
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2"/>
+      <c r="R72" s="2"/>
+      <c r="S72" s="2"/>
+      <c r="T72" s="2"/>
+      <c r="U72" s="2"/>
+      <c r="V72" s="2"/>
+      <c r="W72" s="2"/>
+      <c r="X72" s="2"/>
+      <c r="Y72" s="2"/>
+      <c r="Z72" s="2"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="75">
         <v>1.0</v>
       </c>
-      <c r="B71" s="74" t="s">
-        <v>59</v>
+      <c r="B73" s="76" t="s">
+        <v>61</v>
       </c>
-      <c r="C71" s="75">
+      <c r="C73" s="77">
         <v>1.0</v>
       </c>
-      <c r="D71" s="76"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="77"/>
-      <c r="G71" s="77"/>
-      <c r="H71" s="77"/>
-      <c r="I71" s="77"/>
-      <c r="J71" s="77"/>
-      <c r="K71" s="77"/>
-      <c r="L71" s="77"/>
-      <c r="M71" s="77"/>
-      <c r="N71" s="77"/>
-      <c r="O71" s="77"/>
-      <c r="P71" s="77"/>
-      <c r="Q71" s="77"/>
-      <c r="R71" s="77"/>
-      <c r="S71" s="77"/>
-      <c r="T71" s="77"/>
-      <c r="U71" s="77"/>
-      <c r="V71" s="77"/>
-      <c r="W71" s="77"/>
-      <c r="X71" s="77"/>
-      <c r="Y71" s="77"/>
-      <c r="Z71" s="77"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="27">
+      <c r="D73" s="78"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="79"/>
+      <c r="G73" s="79"/>
+      <c r="H73" s="79"/>
+      <c r="I73" s="79"/>
+      <c r="J73" s="79"/>
+      <c r="K73" s="79"/>
+      <c r="L73" s="79"/>
+      <c r="M73" s="79"/>
+      <c r="N73" s="79"/>
+      <c r="O73" s="79"/>
+      <c r="P73" s="79"/>
+      <c r="Q73" s="79"/>
+      <c r="R73" s="79"/>
+      <c r="S73" s="79"/>
+      <c r="T73" s="79"/>
+      <c r="U73" s="79"/>
+      <c r="V73" s="79"/>
+      <c r="W73" s="79"/>
+      <c r="X73" s="79"/>
+      <c r="Y73" s="79"/>
+      <c r="Z73" s="79"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="29">
         <v>2.0</v>
       </c>
-      <c r="B72" s="12" t="s">
-        <v>60</v>
+      <c r="B74" s="14" t="s">
+        <v>62</v>
       </c>
-      <c r="C72" s="78">
+      <c r="C74" s="80">
         <v>1.0</v>
       </c>
-      <c r="D72" s="79"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="77"/>
-      <c r="G72" s="77"/>
-      <c r="H72" s="77"/>
-      <c r="I72" s="77"/>
-      <c r="J72" s="77"/>
-      <c r="K72" s="77"/>
-      <c r="L72" s="77"/>
-      <c r="M72" s="77"/>
-      <c r="N72" s="77"/>
-      <c r="O72" s="77"/>
-      <c r="P72" s="77"/>
-      <c r="Q72" s="77"/>
-      <c r="R72" s="77"/>
-      <c r="S72" s="77"/>
-      <c r="T72" s="77"/>
-      <c r="U72" s="77"/>
-      <c r="V72" s="77"/>
-      <c r="W72" s="77"/>
-      <c r="X72" s="77"/>
-      <c r="Y72" s="77"/>
-      <c r="Z72" s="77"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="32">
+      <c r="D74" s="81"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="79"/>
+      <c r="G74" s="79"/>
+      <c r="H74" s="79"/>
+      <c r="I74" s="79"/>
+      <c r="J74" s="79"/>
+      <c r="K74" s="79"/>
+      <c r="L74" s="79"/>
+      <c r="M74" s="79"/>
+      <c r="N74" s="79"/>
+      <c r="O74" s="79"/>
+      <c r="P74" s="79"/>
+      <c r="Q74" s="79"/>
+      <c r="R74" s="79"/>
+      <c r="S74" s="79"/>
+      <c r="T74" s="79"/>
+      <c r="U74" s="79"/>
+      <c r="V74" s="79"/>
+      <c r="W74" s="79"/>
+      <c r="X74" s="79"/>
+      <c r="Y74" s="79"/>
+      <c r="Z74" s="79"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="34">
         <v>3.0</v>
       </c>
-      <c r="B73" s="15" t="s">
-        <v>61</v>
+      <c r="B75" s="17" t="s">
+        <v>63</v>
       </c>
-      <c r="C73" s="33">
+      <c r="C75" s="35">
         <v>1.0</v>
       </c>
-      <c r="D73" s="80"/>
-      <c r="E73" s="60"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
-      <c r="O73" s="2"/>
-      <c r="P73" s="2"/>
-      <c r="Q73" s="2"/>
-      <c r="R73" s="2"/>
-      <c r="S73" s="2"/>
-      <c r="T73" s="2"/>
-      <c r="U73" s="2"/>
-      <c r="V73" s="2"/>
-      <c r="W73" s="2"/>
-      <c r="X73" s="2"/>
-      <c r="Y73" s="2"/>
-      <c r="Z73" s="2"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="36"/>
-      <c r="B74" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C74" s="3">
-        <f>SUM(C71:C73)</f>
-        <v>3</v>
-      </c>
-      <c r="D74" s="1">
-        <f>sum(D71:D73)</f>
-        <v>0</v>
-      </c>
-      <c r="E74" s="4"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
-      <c r="L74" s="2"/>
-      <c r="M74" s="2"/>
-      <c r="N74" s="2"/>
-      <c r="O74" s="2"/>
-      <c r="P74" s="2"/>
-      <c r="Q74" s="2"/>
-      <c r="R74" s="2"/>
-      <c r="S74" s="2"/>
-      <c r="T74" s="2"/>
-      <c r="U74" s="2"/>
-      <c r="V74" s="2"/>
-      <c r="W74" s="2"/>
-      <c r="X74" s="2"/>
-      <c r="Y74" s="2"/>
-      <c r="Z74" s="2"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="1"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="4"/>
+      <c r="D75" s="82"/>
+      <c r="E75" s="62"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
@@ -3805,16 +3754,16 @@
       <c r="Z75" s="2"/>
     </row>
     <row r="76">
-      <c r="A76" s="81"/>
-      <c r="B76" s="82" t="s">
-        <v>62</v>
+      <c r="A76" s="38"/>
+      <c r="B76" s="39" t="s">
+        <v>20</v>
       </c>
-      <c r="C76" s="83">
-        <f t="shared" ref="C76:D76" si="2">sum(C18,C27,C35,C48,C55,C67,C74)</f>
-        <v>28</v>
+      <c r="C76" s="3">
+        <f>SUM(C73:C75)</f>
+        <v>3</v>
       </c>
-      <c r="D76" s="84">
-        <f t="shared" si="2"/>
+      <c r="D76" s="1">
+        <f>sum(D73:D75)</f>
         <v>0</v>
       </c>
       <c r="E76" s="4"/>
@@ -3869,10 +3818,18 @@
       <c r="Z77" s="2"/>
     </row>
     <row r="78">
-      <c r="A78" s="1"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="1"/>
+      <c r="A78" s="83"/>
+      <c r="B78" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" s="85">
+        <f t="shared" ref="C78:D78" si="2">sum(C20,C29,C37,C50,C57,C69,C76)</f>
+        <v>28</v>
+      </c>
+      <c r="D78" s="86">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="E78" s="4"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -3896,11 +3853,9 @@
       <c r="Y78" s="2"/>
       <c r="Z78" s="2"/>
     </row>
-    <row r="79" ht="45.75" customHeight="1">
+    <row r="79">
       <c r="A79" s="1"/>
-      <c r="B79" s="85" t="s">
-        <v>63</v>
-      </c>
+      <c r="B79" s="2"/>
       <c r="C79" s="3"/>
       <c r="D79" s="1"/>
       <c r="E79" s="4"/>
@@ -3928,16 +3883,10 @@
     </row>
     <row r="80">
       <c r="A80" s="1"/>
-      <c r="B80" s="86" t="s">
-        <v>64</v>
-      </c>
-      <c r="C80" s="87" t="s">
-        <v>65</v>
-      </c>
-      <c r="D80" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="E80" s="89"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="4"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -3960,16 +3909,14 @@
       <c r="Y80" s="2"/>
       <c r="Z80" s="2"/>
     </row>
-    <row r="81">
+    <row r="81" ht="45.75" customHeight="1">
       <c r="A81" s="1"/>
-      <c r="B81" s="9" t="s">
-        <v>67</v>
+      <c r="B81" s="87" t="s">
+        <v>65</v>
       </c>
-      <c r="C81" s="90">
-        <v>0.5</v>
-      </c>
-      <c r="D81" s="91"/>
-      <c r="E81" s="92"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="4"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -3994,14 +3941,16 @@
     </row>
     <row r="82">
       <c r="A82" s="1"/>
-      <c r="B82" s="12" t="s">
+      <c r="B82" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="C82" s="89" t="s">
+        <v>67</v>
+      </c>
+      <c r="D82" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="C82" s="93">
-        <v>0.5</v>
-      </c>
-      <c r="D82" s="94"/>
-      <c r="E82" s="95"/>
+      <c r="E82" s="91"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
@@ -4029,11 +3978,11 @@
       <c r="B83" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C83" s="93">
-        <v>2.0</v>
+      <c r="C83" s="92">
+        <v>0.5</v>
       </c>
-      <c r="D83" s="94"/>
-      <c r="E83" s="95"/>
+      <c r="D83" s="93"/>
+      <c r="E83" s="94"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
@@ -4058,14 +4007,14 @@
     </row>
     <row r="84">
       <c r="A84" s="1"/>
-      <c r="B84" s="12" t="s">
+      <c r="B84" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C84" s="93">
-        <v>1.0</v>
+      <c r="C84" s="95">
+        <v>0.5</v>
       </c>
-      <c r="D84" s="94"/>
-      <c r="E84" s="95"/>
+      <c r="D84" s="96"/>
+      <c r="E84" s="97"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
@@ -4090,14 +4039,14 @@
     </row>
     <row r="85">
       <c r="A85" s="1"/>
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C85" s="96">
-        <v>1.0</v>
+      <c r="C85" s="95">
+        <v>2.0</v>
       </c>
-      <c r="D85" s="97"/>
-      <c r="E85" s="98"/>
+      <c r="D85" s="96"/>
+      <c r="E85" s="97"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
@@ -4122,18 +4071,14 @@
     </row>
     <row r="86">
       <c r="A86" s="1"/>
-      <c r="B86" s="37" t="s">
-        <v>18</v>
+      <c r="B86" s="14" t="s">
+        <v>72</v>
       </c>
-      <c r="C86" s="3">
-        <f t="shared" ref="C86:D86" si="3">SUM(C81:C85)</f>
-        <v>5</v>
+      <c r="C86" s="95">
+        <v>1.0</v>
       </c>
-      <c r="D86" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E86" s="4"/>
+      <c r="D86" s="96"/>
+      <c r="E86" s="97"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -4158,10 +4103,14 @@
     </row>
     <row r="87">
       <c r="A87" s="1"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="4"/>
+      <c r="B87" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C87" s="98">
+        <v>1.0</v>
+      </c>
+      <c r="D87" s="99"/>
+      <c r="E87" s="100"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -4186,9 +4135,17 @@
     </row>
     <row r="88">
       <c r="A88" s="1"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="1"/>
+      <c r="B88" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C88" s="3">
+        <f t="shared" ref="C88:D88" si="3">SUM(C83:C87)</f>
+        <v>5</v>
+      </c>
+      <c r="D88" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="E88" s="4"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -4242,17 +4199,9 @@
     </row>
     <row r="90">
       <c r="A90" s="1"/>
-      <c r="B90" s="82" t="s">
-        <v>72</v>
-      </c>
-      <c r="C90" s="83">
-        <f>C76</f>
-        <v>28</v>
-      </c>
-      <c r="D90" s="99">
-        <f>D76-D86</f>
-        <v>0</v>
-      </c>
+      <c r="B90" s="2"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="1"/>
       <c r="E90" s="4"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
@@ -4306,9 +4255,17 @@
     </row>
     <row r="92">
       <c r="A92" s="1"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="1"/>
+      <c r="B92" s="84" t="s">
+        <v>74</v>
+      </c>
+      <c r="C92" s="85">
+        <f>C78</f>
+        <v>28</v>
+      </c>
+      <c r="D92" s="101">
+        <f>D78-D88</f>
+        <v>0</v>
+      </c>
       <c r="E92" s="4"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -29980,9 +29937,65 @@
       <c r="Y1008" s="2"/>
       <c r="Z1008" s="2"/>
     </row>
+    <row r="1009">
+      <c r="A1009" s="1"/>
+      <c r="B1009" s="2"/>
+      <c r="C1009" s="3"/>
+      <c r="D1009" s="1"/>
+      <c r="E1009" s="4"/>
+      <c r="F1009" s="2"/>
+      <c r="G1009" s="2"/>
+      <c r="H1009" s="2"/>
+      <c r="I1009" s="2"/>
+      <c r="J1009" s="2"/>
+      <c r="K1009" s="2"/>
+      <c r="L1009" s="2"/>
+      <c r="M1009" s="2"/>
+      <c r="N1009" s="2"/>
+      <c r="O1009" s="2"/>
+      <c r="P1009" s="2"/>
+      <c r="Q1009" s="2"/>
+      <c r="R1009" s="2"/>
+      <c r="S1009" s="2"/>
+      <c r="T1009" s="2"/>
+      <c r="U1009" s="2"/>
+      <c r="V1009" s="2"/>
+      <c r="W1009" s="2"/>
+      <c r="X1009" s="2"/>
+      <c r="Y1009" s="2"/>
+      <c r="Z1009" s="2"/>
+    </row>
+    <row r="1010">
+      <c r="A1010" s="1"/>
+      <c r="B1010" s="2"/>
+      <c r="C1010" s="3"/>
+      <c r="D1010" s="1"/>
+      <c r="E1010" s="4"/>
+      <c r="F1010" s="2"/>
+      <c r="G1010" s="2"/>
+      <c r="H1010" s="2"/>
+      <c r="I1010" s="2"/>
+      <c r="J1010" s="2"/>
+      <c r="K1010" s="2"/>
+      <c r="L1010" s="2"/>
+      <c r="M1010" s="2"/>
+      <c r="N1010" s="2"/>
+      <c r="O1010" s="2"/>
+      <c r="P1010" s="2"/>
+      <c r="Q1010" s="2"/>
+      <c r="R1010" s="2"/>
+      <c r="S1010" s="2"/>
+      <c r="T1010" s="2"/>
+      <c r="U1010" s="2"/>
+      <c r="V1010" s="2"/>
+      <c r="W1010" s="2"/>
+      <c r="X1010" s="2"/>
+      <c r="Y1010" s="2"/>
+      <c r="Z1010" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E2:E7"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>